<commit_message>
Fix broken meta fields
For #6005
</commit_message>
<xml_diff>
--- a/config/default/forms/app/pnc_danger_sign_follow_up_mother.xlsx
+++ b/config/default/forms/app/pnc_danger_sign_follow_up_mother.xlsx
@@ -16,6 +16,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="287">
   <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -25,6 +31,24 @@
     <t>label::en</t>
   </si>
   <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>default_language</t>
+  </si>
+  <si>
     <t>label::hi</t>
   </si>
   <si>
@@ -118,139 +142,148 @@
     <t>cht::notes</t>
   </si>
   <si>
-    <t>form_title</t>
+    <t>PNC danger sign follow-up - mother</t>
   </si>
   <si>
     <t>begin group</t>
   </si>
   <si>
+    <t>pnc_danger_sign_follow_up_mother</t>
+  </si>
+  <si>
     <t>inputs</t>
   </si>
   <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>default_language</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>PNC danger sign follow-up - mother</t>
-  </si>
-  <si>
-    <t>pnc_danger_sign_follow_up_mother</t>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
   </si>
   <si>
     <t>pages</t>
   </si>
   <si>
-    <t>./source = 'user'</t>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>delivery_uuid</t>
+  </si>
+  <si>
+    <t>Delivery Report ID</t>
   </si>
   <si>
     <t>data</t>
   </si>
   <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>hidden</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>source_id</t>
-  </si>
-  <si>
-    <t>Source ID</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
-    <t>delivery_uuid</t>
-  </si>
-  <si>
-    <t>Delivery Report ID</t>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
   </si>
   <si>
     <t>yes_no</t>
   </si>
   <si>
+    <t>Parent ID</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>db:person</t>
-  </si>
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>What is the patient's name?</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>Short Name</t>
-  </si>
-  <si>
     <t>translate_woman_label</t>
   </si>
   <si>
+    <t>chw_name</t>
+  </si>
+  <si>
+    <t>CHW name</t>
+  </si>
+  <si>
     <t>woman</t>
   </si>
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>the woman</t>
   </si>
   <si>
-    <t>Patient ID</t>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>CHW phone</t>
   </si>
   <si>
     <t>translate_woman_start_label</t>
@@ -262,39 +295,6 @@
     <t>The woman</t>
   </si>
   <si>
-    <t>date_of_birth</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>Parent ID</t>
-  </si>
-  <si>
-    <t>chw_name</t>
-  </si>
-  <si>
-    <t>CHW name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>CHW phone</t>
-  </si>
-  <si>
     <t>end group</t>
   </si>
   <si>
@@ -325,12 +325,45 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>lmp_approximations</t>
+  </si>
+  <si>
+    <t>upto_2_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 2 Months Ago</t>
+  </si>
+  <si>
+    <t>upto_3_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 3 Months Ago</t>
+  </si>
+  <si>
+    <t>upto_4_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 4 Months Ago</t>
+  </si>
+  <si>
     <t>patient_short_name</t>
   </si>
   <si>
+    <t>between_5_and_6_months_ago</t>
+  </si>
+  <si>
+    <t>Between 5 And 6 Months Ago</t>
+  </si>
+  <si>
     <t>coalesce(../inputs/contact/short_name, ../danger_signs/custom_translations/custom_woman_label)</t>
   </si>
   <si>
+    <t>between_7_and_8_months_ago</t>
+  </si>
+  <si>
+    <t>Between 7 And 8 Months Ago</t>
+  </si>
+  <si>
     <t>patient_short_name_start</t>
   </si>
   <si>
@@ -343,57 +376,24 @@
     <t>date-time(floor(decimal-date-time(today())) + 3)</t>
   </si>
   <si>
-    <t>lmp_approximations</t>
-  </si>
-  <si>
-    <t>upto_2_months_ago</t>
-  </si>
-  <si>
-    <t>Upto 2 Months Ago</t>
-  </si>
-  <si>
-    <t>upto_3_months_ago</t>
+    <t>trimester1_choices</t>
+  </si>
+  <si>
+    <t>eat_extra_meal</t>
+  </si>
+  <si>
+    <t>Eat a balanced diet daily, and one extra meal and water to help the baby grow well and for you to remain strong and healthy</t>
   </si>
   <si>
     <t>t_danger_signs_referral_follow_up</t>
   </si>
   <si>
-    <t>Upto 3 Months Ago</t>
+    <t>take_iron_and_folic_acid</t>
   </si>
   <si>
     <t>../danger_signs/r_danger_sign_present</t>
   </si>
   <si>
-    <t>upto_4_months_ago</t>
-  </si>
-  <si>
-    <t>Upto 4 Months Ago</t>
-  </si>
-  <si>
-    <t>between_5_and_6_months_ago</t>
-  </si>
-  <si>
-    <t>Between 5 And 6 Months Ago</t>
-  </si>
-  <si>
-    <t>between_7_and_8_months_ago</t>
-  </si>
-  <si>
-    <t>Between 7 And 8 Months Ago</t>
-  </si>
-  <si>
-    <t>trimester1_choices</t>
-  </si>
-  <si>
-    <t>eat_extra_meal</t>
-  </si>
-  <si>
-    <t>Eat a balanced diet daily, and one extra meal and water to help the baby grow well and for you to remain strong and healthy</t>
-  </si>
-  <si>
-    <t>take_iron_and_folic_acid</t>
-  </si>
-  <si>
     <t>Take iron and folic acid tablets</t>
   </si>
   <si>
@@ -409,24 +409,24 @@
     <t>Sleep under an insecticide treated bednet</t>
   </si>
   <si>
+    <t>go_for_anc_visit</t>
+  </si>
+  <si>
+    <t>Go for an antenantal care visit as soon as you know you are pregnant, and at least four times during the pregnancy</t>
+  </si>
+  <si>
+    <t>develop_birth_plan</t>
+  </si>
+  <si>
+    <t>Develop a birth plan to ensure readiness for the arrival of the unborn baby</t>
+  </si>
+  <si>
     <t>danger_signs</t>
   </si>
   <si>
     <t>Danger Sign Follow-up - Mother</t>
   </si>
   <si>
-    <t>go_for_anc_visit</t>
-  </si>
-  <si>
-    <t>Go for an antenantal care visit as soon as you know you are pregnant, and at least four times during the pregnancy</t>
-  </si>
-  <si>
-    <t>develop_birth_plan</t>
-  </si>
-  <si>
-    <t>Develop a birth plan to ensure readiness for the arrival of the unborn baby</t>
-  </si>
-  <si>
     <t>trimester2_choices</t>
   </si>
   <si>
@@ -445,18 +445,18 @@
     <t>Is she still experiencing any danger signs?</t>
   </si>
   <si>
+    <t>couselling_on_exclusive_breastfeeding</t>
+  </si>
+  <si>
+    <t>Give your baby breast milk only (exclusive breastfeeding) for the first six months and continue breastfeeding for the first two years for good health</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
-    <t>couselling_on_exclusive_breastfeeding</t>
-  </si>
-  <si>
     <t>danger_signs_question_note</t>
   </si>
   <si>
-    <t>Give your baby breast milk only (exclusive breastfeeding) for the first six months and continue breastfeeding for the first two years for good health</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please indicate which danger signs ${patient_short_name} is experiencing. </t>
   </si>
   <si>
@@ -472,36 +472,36 @@
     <t>Heart condition</t>
   </si>
   <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
     <t>fever</t>
   </si>
   <si>
     <t>Fever</t>
   </si>
   <si>
-    <t>asthma</t>
-  </si>
-  <si>
-    <t>Asthma</t>
-  </si>
-  <si>
     <t>high_blood_pressure</t>
   </si>
   <si>
     <t>High blood pressure</t>
   </si>
   <si>
+    <t>known_diabetes</t>
+  </si>
+  <si>
+    <t>Known diabetes</t>
+  </si>
+  <si>
     <t>severe_headache</t>
   </si>
   <si>
     <t>Severe headache</t>
   </si>
   <si>
-    <t>known_diabetes</t>
-  </si>
-  <si>
-    <t>Known diabetes</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -514,28 +514,28 @@
     <t>Vaginal bleeding</t>
   </si>
   <si>
+    <t>hiv_statuses</t>
+  </si>
+  <si>
+    <t>known</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>vaginal_discharge</t>
   </si>
   <si>
-    <t>hiv_statuses</t>
-  </si>
-  <si>
-    <t>known</t>
-  </si>
-  <si>
     <t>Foul smelling vaginal discharge</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>fp_methods</t>
   </si>
   <si>
     <t>convulsion</t>
   </si>
   <si>
     <t>Convulsions</t>
-  </si>
-  <si>
-    <t>fp_methods</t>
   </si>
   <si>
     <t>r_danger_sign_present</t>
@@ -570,66 +570,66 @@
     <t>../danger_sign_present = 'yes' or ../r_danger_sign_present = 'yes'</t>
   </si>
   <si>
+    <t>Combined oral contraceptives</t>
+  </si>
+  <si>
+    <t>Progesterone only pills</t>
+  </si>
+  <si>
     <t>refer_patient_note_2</t>
   </si>
   <si>
     <t xml:space="preserve">Please advise her to do so and accompany her if possible. </t>
   </si>
   <si>
+    <t>Injectibles</t>
+  </si>
+  <si>
+    <t>Implants (1 rod)</t>
+  </si>
+  <si>
+    <t>Implants (2 rods)</t>
+  </si>
+  <si>
     <t>custom_translations</t>
   </si>
   <si>
-    <t>Combined oral contraceptives</t>
-  </si>
-  <si>
-    <t>Progesterone only pills</t>
-  </si>
-  <si>
-    <t>Injectibles</t>
+    <t>IUD</t>
+  </si>
+  <si>
+    <t>Condoms</t>
+  </si>
+  <si>
+    <t>Tubal ligation</t>
+  </si>
+  <si>
+    <t>Cycle beads</t>
   </si>
   <si>
     <t>select_one translate_woman_label</t>
   </si>
   <si>
-    <t>Implants (1 rod)</t>
-  </si>
-  <si>
     <t>custom_woman_label_translator</t>
   </si>
   <si>
-    <t>Implants (2 rods)</t>
-  </si>
-  <si>
     <t>"woman"</t>
   </si>
   <si>
-    <t>IUD</t>
-  </si>
-  <si>
-    <t>Condoms</t>
+    <t>reasons_not_on_fp</t>
+  </si>
+  <si>
+    <t>Wants to get pregnant</t>
   </si>
   <si>
     <t>custom_woman_label</t>
   </si>
   <si>
-    <t>Tubal ligation</t>
-  </si>
-  <si>
-    <t>Cycle beads</t>
+    <t>Did not want FP</t>
   </si>
   <si>
     <t>jr:choice-name(${custom_woman_label_translator},'${custom_woman_label_translator}')</t>
   </si>
   <si>
-    <t>reasons_not_on_fp</t>
-  </si>
-  <si>
-    <t>Wants to get pregnant</t>
-  </si>
-  <si>
-    <t>Did not want FP</t>
-  </si>
-  <si>
     <t>follow_up_methods</t>
   </si>
   <si>
@@ -645,16 +645,19 @@
     <t>In person</t>
   </si>
   <si>
+    <t>"woman-start"</t>
+  </si>
+  <si>
+    <t>custom_woman_start_label</t>
+  </si>
+  <si>
     <t>by_phone</t>
   </si>
   <si>
     <t>By phone</t>
   </si>
   <si>
-    <t>"woman-start"</t>
-  </si>
-  <si>
-    <t>custom_woman_start_label</t>
+    <t>jr:choice-name(${custom_woman_start_label_translator},'${custom_woman_start_label_translator}')</t>
   </si>
   <si>
     <t>reasons_for_missing_visit</t>
@@ -666,9 +669,6 @@
     <t>She was not reminded</t>
   </si>
   <si>
-    <t>jr:choice-name(${custom_woman_start_label_translator},'${custom_woman_start_label_translator}')</t>
-  </si>
-  <si>
     <t>travelled</t>
   </si>
   <si>
@@ -852,37 +852,37 @@
     <t>__patient_uuid</t>
   </si>
   <si>
-    <t>../../inputs/contact/_id</t>
+    <t>../../../inputs/contact/_id</t>
   </si>
   <si>
     <t>__patient_id</t>
   </si>
   <si>
-    <t>../../inputs/contact/patient_id</t>
+    <t>../../../inputs/contact/patient_id</t>
   </si>
   <si>
     <t>__household_uuid</t>
   </si>
   <si>
-    <t>../../inputs/contact/parent/_id</t>
+    <t>../../../inputs/contact/parent/_id</t>
   </si>
   <si>
     <t>__source</t>
   </si>
   <si>
-    <t>../../inputs/source</t>
+    <t>../../../inputs/source</t>
   </si>
   <si>
     <t>__source_id</t>
   </si>
   <si>
-    <t>../../inputs/source_id</t>
+    <t>../../../inputs/source_id</t>
   </si>
   <si>
     <t>__delivery_uuid</t>
   </si>
   <si>
-    <t>../../inputs/delivery_uuid</t>
+    <t>../../../inputs/delivery_uuid</t>
   </si>
 </sst>
 </file>
@@ -900,6 +900,11 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
     </font>
     <font>
       <b/>
@@ -908,11 +913,6 @@
       <name val="Calibri"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -953,6 +953,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
@@ -961,12 +967,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1025,14 +1025,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF8E7CC3"/>
+        <bgColor rgb="FF8E7CC3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8E7CC3"/>
-        <bgColor rgb="FF8E7CC3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1046,105 +1046,105 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="12" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="13" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="13" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -1154,28 +1154,28 @@
     <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="15" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1242,120 +1242,120 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
+      <c r="AA1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>36</v>
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1365,10 +1365,10 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -1396,14 +1396,14 @@
       <c r="AJ2" s="12"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1432,7 +1432,7 @@
       <c r="AB3" s="9"/>
       <c r="AC3" s="9"/>
       <c r="AD3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE3" s="9"/>
       <c r="AF3" s="9"/>
@@ -1442,14 +1442,14 @@
       <c r="AJ3" s="12"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1486,14 +1486,14 @@
       <c r="AJ4" s="12"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>59</v>
+      <c r="A5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1530,14 +1530,14 @@
       <c r="AJ5" s="12"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1574,14 +1574,14 @@
       <c r="AJ6" s="12"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>66</v>
+      <c r="A7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1592,7 +1592,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -1620,14 +1620,14 @@
       <c r="AJ7" s="12"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
+      <c r="A8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1664,14 +1664,14 @@
       <c r="AJ8" s="12"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>73</v>
+      <c r="A9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1708,14 +1708,14 @@
       <c r="AJ9" s="12"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>76</v>
+      <c r="A10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1752,14 +1752,14 @@
       <c r="AJ10" s="12"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>82</v>
+      <c r="A11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1798,14 +1798,14 @@
       <c r="AJ11" s="12"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>84</v>
+      <c r="A12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1842,14 +1842,14 @@
       <c r="AJ12" s="12"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>86</v>
+      <c r="A13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1886,14 +1886,14 @@
       <c r="AJ13" s="12"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>66</v>
+      <c r="A14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1925,19 +1925,19 @@
       <c r="AE14" s="9"/>
       <c r="AF14" s="9"/>
       <c r="AG14" s="9"/>
-      <c r="AH14" s="29"/>
-      <c r="AI14" s="29"/>
-      <c r="AJ14" s="29"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>86</v>
+      <c r="A15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -1974,14 +1974,14 @@
       <c r="AJ15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
+      <c r="A16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -2018,14 +2018,14 @@
       <c r="AJ16" s="12"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>89</v>
+      <c r="A17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -2062,14 +2062,14 @@
       <c r="AJ17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
+      <c r="A18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -2106,11 +2106,11 @@
       <c r="AJ18" s="12"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>63</v>
+      <c r="B19" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2148,11 +2148,11 @@
       <c r="AJ19" s="12"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>86</v>
+      <c r="B20" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2190,11 +2190,11 @@
       <c r="AJ20" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>86</v>
+      <c r="B21" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2232,11 +2232,11 @@
       <c r="AJ21" s="12"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>63</v>
+      <c r="B22" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2274,11 +2274,11 @@
       <c r="AJ22" s="12"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>36</v>
+      <c r="B23" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2362,7 +2362,7 @@
       <c r="AD25" s="33"/>
       <c r="AE25" s="33"/>
       <c r="AF25" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG25" s="33"/>
       <c r="AH25" s="35"/>
@@ -2410,7 +2410,7 @@
       <c r="AD26" s="33"/>
       <c r="AE26" s="33"/>
       <c r="AF26" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG26" s="33"/>
       <c r="AH26" s="35"/>
@@ -2422,7 +2422,7 @@
         <v>94</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
@@ -2434,7 +2434,7 @@
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
       <c r="J27" s="33" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K27" s="33"/>
       <c r="L27" s="33"/>
@@ -2460,7 +2460,7 @@
       <c r="AD27" s="33"/>
       <c r="AE27" s="33"/>
       <c r="AF27" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG27" s="33"/>
       <c r="AH27" s="35"/>
@@ -2508,7 +2508,7 @@
       <c r="AD28" s="33"/>
       <c r="AE28" s="33"/>
       <c r="AF28" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG28" s="33"/>
       <c r="AH28" s="35"/>
@@ -2520,7 +2520,7 @@
         <v>94</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>96</v>
@@ -2543,7 +2543,7 @@
       <c r="S29" s="33"/>
       <c r="T29" s="33"/>
       <c r="U29" s="34" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="V29" s="33"/>
       <c r="W29" s="33"/>
@@ -2556,7 +2556,7 @@
       <c r="AD29" s="33"/>
       <c r="AE29" s="33"/>
       <c r="AF29" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG29" s="33"/>
       <c r="AH29" s="35"/>
@@ -2568,7 +2568,7 @@
         <v>94</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>96</v>
@@ -2591,7 +2591,7 @@
       <c r="S30" s="33"/>
       <c r="T30" s="33"/>
       <c r="U30" s="34" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
@@ -2604,7 +2604,7 @@
       <c r="AD30" s="33"/>
       <c r="AE30" s="33"/>
       <c r="AF30" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG30" s="33"/>
       <c r="AH30" s="35"/>
@@ -2616,7 +2616,7 @@
         <v>94</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C31" s="34" t="s">
         <v>96</v>
@@ -2639,7 +2639,7 @@
       <c r="S31" s="33"/>
       <c r="T31" s="33"/>
       <c r="U31" s="34" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="V31" s="33"/>
       <c r="W31" s="33"/>
@@ -2652,7 +2652,7 @@
       <c r="AD31" s="33"/>
       <c r="AE31" s="33"/>
       <c r="AF31" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG31" s="33"/>
       <c r="AH31" s="37"/>
@@ -2664,7 +2664,7 @@
         <v>94</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>96</v>
@@ -2687,7 +2687,7 @@
       <c r="S32" s="33"/>
       <c r="T32" s="33"/>
       <c r="U32" s="34" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="V32" s="33"/>
       <c r="W32" s="33"/>
@@ -2700,7 +2700,7 @@
       <c r="AD32" s="33"/>
       <c r="AE32" s="33"/>
       <c r="AF32" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG32" s="33"/>
       <c r="AH32" s="37"/>
@@ -2719,13 +2719,13 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="39" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
@@ -2736,7 +2736,7 @@
       <c r="J34" s="41"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M34" s="41"/>
       <c r="N34" s="41"/>
@@ -2780,7 +2780,7 @@
       <c r="H35" s="41"/>
       <c r="I35" s="41"/>
       <c r="J35" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K35" s="41"/>
       <c r="L35" s="41"/>
@@ -2826,7 +2826,7 @@
       <c r="H36" s="41"/>
       <c r="I36" s="41"/>
       <c r="J36" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K36" s="41"/>
       <c r="L36" s="41"/>
@@ -2857,10 +2857,10 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>147</v>
@@ -2896,7 +2896,7 @@
       <c r="AD37" s="41"/>
       <c r="AE37" s="41"/>
       <c r="AF37" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG37" s="41"/>
       <c r="AH37" s="42"/>
@@ -2908,10 +2908,10 @@
         <v>138</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
@@ -2920,7 +2920,7 @@
       <c r="H38" s="41"/>
       <c r="I38" s="41"/>
       <c r="J38" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K38" s="40" t="s">
         <v>148</v>
@@ -2956,10 +2956,10 @@
         <v>138</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
@@ -2968,7 +2968,7 @@
       <c r="H39" s="41"/>
       <c r="I39" s="41"/>
       <c r="J39" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K39" s="40" t="s">
         <v>148</v>
@@ -3016,7 +3016,7 @@
       <c r="H40" s="41"/>
       <c r="I40" s="41"/>
       <c r="J40" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K40" s="40" t="s">
         <v>148</v>
@@ -3052,10 +3052,10 @@
         <v>138</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
@@ -3064,7 +3064,7 @@
       <c r="H41" s="41"/>
       <c r="I41" s="41"/>
       <c r="J41" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K41" s="40" t="s">
         <v>148</v>
@@ -3100,10 +3100,10 @@
         <v>138</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
@@ -3112,7 +3112,7 @@
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K42" s="40" t="s">
         <v>148</v>
@@ -3184,7 +3184,7 @@
       <c r="AD43" s="41"/>
       <c r="AE43" s="41"/>
       <c r="AF43" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG43" s="41"/>
       <c r="AH43" s="42"/>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B44" s="39" t="s">
         <v>176</v>
@@ -3232,7 +3232,7 @@
       <c r="AD44" s="41"/>
       <c r="AE44" s="41"/>
       <c r="AF44" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG44" s="41"/>
       <c r="AH44" s="44"/>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B45" s="39" t="s">
         <v>179</v>
@@ -3280,7 +3280,7 @@
       <c r="AD45" s="41"/>
       <c r="AE45" s="41"/>
       <c r="AF45" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG45" s="41"/>
       <c r="AH45" s="44"/>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D46" s="41"/>
       <c r="E46" s="41"/>
@@ -3328,7 +3328,7 @@
       <c r="AD46" s="41"/>
       <c r="AE46" s="41"/>
       <c r="AF46" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG46" s="41"/>
       <c r="AH46" s="42"/>
@@ -3337,10 +3337,10 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="39" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>96</v>
@@ -3354,7 +3354,7 @@
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
       <c r="L47" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M47" s="41"/>
       <c r="N47" s="41"/>
@@ -3376,7 +3376,7 @@
       <c r="AD47" s="41"/>
       <c r="AE47" s="41"/>
       <c r="AF47" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG47" s="41"/>
       <c r="AH47" s="45"/>
@@ -3385,10 +3385,10 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="39" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>96</v>
@@ -3411,7 +3411,7 @@
       <c r="S48" s="41"/>
       <c r="T48" s="41"/>
       <c r="U48" s="40" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="V48" s="41"/>
       <c r="W48" s="41"/>
@@ -3434,7 +3434,7 @@
         <v>94</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>96</v>
@@ -3457,7 +3457,7 @@
       <c r="S49" s="41"/>
       <c r="T49" s="41"/>
       <c r="U49" s="40" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="V49" s="41"/>
       <c r="W49" s="41"/>
@@ -3503,7 +3503,7 @@
       <c r="S50" s="41"/>
       <c r="T50" s="41"/>
       <c r="U50" s="40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="V50" s="41"/>
       <c r="W50" s="41"/>
@@ -3526,7 +3526,7 @@
         <v>94</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>96</v>
@@ -3549,7 +3549,7 @@
       <c r="S51" s="41"/>
       <c r="T51" s="41"/>
       <c r="U51" s="40" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="V51" s="41"/>
       <c r="W51" s="41"/>
@@ -3655,16 +3655,16 @@
       <c r="F54" s="30"/>
       <c r="AF54" s="30"/>
       <c r="AG54" s="30"/>
-      <c r="AH54" s="48"/>
-      <c r="AI54" s="48"/>
-      <c r="AJ54" s="48"/>
+      <c r="AH54" s="47"/>
+      <c r="AI54" s="47"/>
+      <c r="AJ54" s="47"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="49" t="s">
-        <v>49</v>
+      <c r="A55" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="48" t="s">
+        <v>58</v>
       </c>
       <c r="C55" s="50" t="s">
         <v>96</v>
@@ -3678,7 +3678,7 @@
       <c r="J55" s="51"/>
       <c r="K55" s="51"/>
       <c r="L55" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M55" s="51"/>
       <c r="N55" s="51"/>
@@ -3700,7 +3700,7 @@
       <c r="AD55" s="51"/>
       <c r="AE55" s="51"/>
       <c r="AF55" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG55" s="50"/>
       <c r="AH55" s="53"/>
@@ -3708,7 +3708,7 @@
       <c r="AJ55" s="53"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="54" t="s">
@@ -3754,7 +3754,7 @@
       <c r="AJ56" s="53"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="54" t="s">
@@ -3800,7 +3800,7 @@
       <c r="AJ57" s="53"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B58" s="54" t="s">
@@ -3846,7 +3846,7 @@
       <c r="AJ58" s="53"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B59" s="54" t="s">
@@ -3892,7 +3892,7 @@
       <c r="AJ59" s="53"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B60" s="54" t="s">
@@ -3938,7 +3938,7 @@
       <c r="AJ60" s="53"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B61" s="54" t="s">
@@ -3984,7 +3984,7 @@
       <c r="AJ61" s="53"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B62" s="54" t="s">
@@ -4030,7 +4030,7 @@
       <c r="AJ62" s="53"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B63" s="54" t="s">
@@ -4077,7 +4077,7 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="56" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B64" s="56" t="s">
         <v>274</v>
@@ -4120,7 +4120,7 @@
       <c r="AJ64" s="53"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B65" s="54" t="s">
@@ -4144,7 +4144,7 @@
       <c r="R65" s="51"/>
       <c r="S65" s="51"/>
       <c r="T65" s="51"/>
-      <c r="U65" s="50" t="s">
+      <c r="U65" s="53" t="s">
         <v>276</v>
       </c>
       <c r="V65" s="51"/>
@@ -4164,7 +4164,7 @@
       <c r="AJ65" s="53"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B66" s="54" t="s">
@@ -4188,7 +4188,7 @@
       <c r="R66" s="51"/>
       <c r="S66" s="51"/>
       <c r="T66" s="51"/>
-      <c r="U66" s="50" t="s">
+      <c r="U66" s="53" t="s">
         <v>278</v>
       </c>
       <c r="V66" s="51"/>
@@ -4208,7 +4208,7 @@
       <c r="AJ66" s="53"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B67" s="54" t="s">
@@ -4232,7 +4232,7 @@
       <c r="R67" s="51"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
-      <c r="U67" s="50" t="s">
+      <c r="U67" s="53" t="s">
         <v>280</v>
       </c>
       <c r="V67" s="51"/>
@@ -4252,7 +4252,7 @@
       <c r="AJ67" s="53"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B68" s="54" t="s">
@@ -4276,7 +4276,7 @@
       <c r="R68" s="51"/>
       <c r="S68" s="51"/>
       <c r="T68" s="51"/>
-      <c r="U68" s="50" t="s">
+      <c r="U68" s="53" t="s">
         <v>282</v>
       </c>
       <c r="V68" s="51"/>
@@ -4296,7 +4296,7 @@
       <c r="AJ68" s="53"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="49" t="s">
+      <c r="A69" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B69" s="54" t="s">
@@ -4320,7 +4320,7 @@
       <c r="R69" s="51"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
-      <c r="U69" s="50" t="s">
+      <c r="U69" s="53" t="s">
         <v>284</v>
       </c>
       <c r="V69" s="51"/>
@@ -4340,7 +4340,7 @@
       <c r="AJ69" s="53"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B70" s="54" t="s">
@@ -4364,7 +4364,7 @@
       <c r="R70" s="51"/>
       <c r="S70" s="51"/>
       <c r="T70" s="51"/>
-      <c r="U70" s="50" t="s">
+      <c r="U70" s="52" t="s">
         <v>286</v>
       </c>
       <c r="V70" s="51"/>
@@ -4430,7 +4430,7 @@
         <v>93</v>
       </c>
       <c r="B72" s="56" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C72" s="53"/>
       <c r="D72" s="57"/>
@@ -4495,56 +4495,56 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -4568,13 +4568,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -4597,9 +4597,9 @@
       <c r="V3" s="25"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -4621,25 +4621,25 @@
       <c r="V4" s="25"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>77</v>
+      <c r="A5" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>81</v>
+      <c r="A6" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -4850,87 +4850,87 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11">
         <f>NOW()</f>
-        <v>43747.52795</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="10" t="s">
+        <v>43748.59599</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
+      <c r="E2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -4955,57 +4955,57 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -5030,13 +5030,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -5086,13 +5086,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
@@ -5117,13 +5117,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
@@ -5148,13 +5148,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>117</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
@@ -5179,13 +5179,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -5210,13 +5210,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -5266,13 +5266,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -5297,10 +5297,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>126</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>127</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>129</v>
@@ -5390,13 +5390,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -5421,13 +5421,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -5480,10 +5480,10 @@
         <v>137</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -5511,7 +5511,7 @@
         <v>137</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>126</v>
@@ -5604,10 +5604,10 @@
         <v>137</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
@@ -5635,10 +5635,10 @@
         <v>137</v>
       </c>
       <c r="B23" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="25" t="s">
         <v>144</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
@@ -5722,10 +5722,10 @@
         <v>149</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
@@ -5784,10 +5784,10 @@
         <v>149</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>168</v>
-      </c>
       <c r="C31" s="25" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -5899,13 +5899,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -5955,115 +5955,115 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B43" t="s">
         <v>162</v>
@@ -6080,26 +6080,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -6109,82 +6109,82 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
-      <c r="T48" s="14"/>
-      <c r="U48" s="14"/>
-      <c r="V48" s="14"/>
-      <c r="W48" s="14"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
+      <c r="B49" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
     </row>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C51" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B52" t="s">
         <v>215</v>
@@ -6195,7 +6195,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
         <v>217</v>
@@ -6206,7 +6206,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s">
         <v>219</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B55" t="s">
         <v>221</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
         <v>162</v>
@@ -6239,102 +6239,102 @@
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="27" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="27" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="27" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="27" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="27" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="27" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="27" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="27" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="27" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6369,8 +6369,8 @@
       <c r="B72" t="s">
         <v>247</v>
       </c>
-      <c r="C72" s="47" t="s">
-        <v>200</v>
+      <c r="C72" s="49" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Fix broken meta fields (#6014)
#6005

(cherry picked from commit 6883b98d08a0ac641350e35fafa5f7ceac088957)
</commit_message>
<xml_diff>
--- a/config/default/forms/app/pnc_danger_sign_follow_up_mother.xlsx
+++ b/config/default/forms/app/pnc_danger_sign_follow_up_mother.xlsx
@@ -16,6 +16,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="287">
   <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -25,6 +31,24 @@
     <t>label::en</t>
   </si>
   <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>default_language</t>
+  </si>
+  <si>
     <t>label::hi</t>
   </si>
   <si>
@@ -118,139 +142,148 @@
     <t>cht::notes</t>
   </si>
   <si>
-    <t>form_title</t>
+    <t>PNC danger sign follow-up - mother</t>
   </si>
   <si>
     <t>begin group</t>
   </si>
   <si>
+    <t>pnc_danger_sign_follow_up_mother</t>
+  </si>
+  <si>
     <t>inputs</t>
   </si>
   <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>default_language</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>PNC danger sign follow-up - mother</t>
-  </si>
-  <si>
-    <t>pnc_danger_sign_follow_up_mother</t>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
   </si>
   <si>
     <t>pages</t>
   </si>
   <si>
-    <t>./source = 'user'</t>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>delivery_uuid</t>
+  </si>
+  <si>
+    <t>Delivery Report ID</t>
   </si>
   <si>
     <t>data</t>
   </si>
   <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>hidden</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>source_id</t>
-  </si>
-  <si>
-    <t>Source ID</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
-    <t>delivery_uuid</t>
-  </si>
-  <si>
-    <t>Delivery Report ID</t>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
   </si>
   <si>
     <t>yes_no</t>
   </si>
   <si>
+    <t>Parent ID</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>db:person</t>
-  </si>
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>What is the patient's name?</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>Short Name</t>
-  </si>
-  <si>
     <t>translate_woman_label</t>
   </si>
   <si>
+    <t>chw_name</t>
+  </si>
+  <si>
+    <t>CHW name</t>
+  </si>
+  <si>
     <t>woman</t>
   </si>
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>the woman</t>
   </si>
   <si>
-    <t>Patient ID</t>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>CHW phone</t>
   </si>
   <si>
     <t>translate_woman_start_label</t>
@@ -262,39 +295,6 @@
     <t>The woman</t>
   </si>
   <si>
-    <t>date_of_birth</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>Parent ID</t>
-  </si>
-  <si>
-    <t>chw_name</t>
-  </si>
-  <si>
-    <t>CHW name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>CHW phone</t>
-  </si>
-  <si>
     <t>end group</t>
   </si>
   <si>
@@ -325,12 +325,45 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>lmp_approximations</t>
+  </si>
+  <si>
+    <t>upto_2_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 2 Months Ago</t>
+  </si>
+  <si>
+    <t>upto_3_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 3 Months Ago</t>
+  </si>
+  <si>
+    <t>upto_4_months_ago</t>
+  </si>
+  <si>
+    <t>Upto 4 Months Ago</t>
+  </si>
+  <si>
     <t>patient_short_name</t>
   </si>
   <si>
+    <t>between_5_and_6_months_ago</t>
+  </si>
+  <si>
+    <t>Between 5 And 6 Months Ago</t>
+  </si>
+  <si>
     <t>coalesce(../inputs/contact/short_name, ../danger_signs/custom_translations/custom_woman_label)</t>
   </si>
   <si>
+    <t>between_7_and_8_months_ago</t>
+  </si>
+  <si>
+    <t>Between 7 And 8 Months Ago</t>
+  </si>
+  <si>
     <t>patient_short_name_start</t>
   </si>
   <si>
@@ -343,57 +376,24 @@
     <t>date-time(floor(decimal-date-time(today())) + 3)</t>
   </si>
   <si>
-    <t>lmp_approximations</t>
-  </si>
-  <si>
-    <t>upto_2_months_ago</t>
-  </si>
-  <si>
-    <t>Upto 2 Months Ago</t>
-  </si>
-  <si>
-    <t>upto_3_months_ago</t>
+    <t>trimester1_choices</t>
+  </si>
+  <si>
+    <t>eat_extra_meal</t>
+  </si>
+  <si>
+    <t>Eat a balanced diet daily, and one extra meal and water to help the baby grow well and for you to remain strong and healthy</t>
   </si>
   <si>
     <t>t_danger_signs_referral_follow_up</t>
   </si>
   <si>
-    <t>Upto 3 Months Ago</t>
+    <t>take_iron_and_folic_acid</t>
   </si>
   <si>
     <t>../danger_signs/r_danger_sign_present</t>
   </si>
   <si>
-    <t>upto_4_months_ago</t>
-  </si>
-  <si>
-    <t>Upto 4 Months Ago</t>
-  </si>
-  <si>
-    <t>between_5_and_6_months_ago</t>
-  </si>
-  <si>
-    <t>Between 5 And 6 Months Ago</t>
-  </si>
-  <si>
-    <t>between_7_and_8_months_ago</t>
-  </si>
-  <si>
-    <t>Between 7 And 8 Months Ago</t>
-  </si>
-  <si>
-    <t>trimester1_choices</t>
-  </si>
-  <si>
-    <t>eat_extra_meal</t>
-  </si>
-  <si>
-    <t>Eat a balanced diet daily, and one extra meal and water to help the baby grow well and for you to remain strong and healthy</t>
-  </si>
-  <si>
-    <t>take_iron_and_folic_acid</t>
-  </si>
-  <si>
     <t>Take iron and folic acid tablets</t>
   </si>
   <si>
@@ -409,24 +409,24 @@
     <t>Sleep under an insecticide treated bednet</t>
   </si>
   <si>
+    <t>go_for_anc_visit</t>
+  </si>
+  <si>
+    <t>Go for an antenantal care visit as soon as you know you are pregnant, and at least four times during the pregnancy</t>
+  </si>
+  <si>
+    <t>develop_birth_plan</t>
+  </si>
+  <si>
+    <t>Develop a birth plan to ensure readiness for the arrival of the unborn baby</t>
+  </si>
+  <si>
     <t>danger_signs</t>
   </si>
   <si>
     <t>Danger Sign Follow-up - Mother</t>
   </si>
   <si>
-    <t>go_for_anc_visit</t>
-  </si>
-  <si>
-    <t>Go for an antenantal care visit as soon as you know you are pregnant, and at least four times during the pregnancy</t>
-  </si>
-  <si>
-    <t>develop_birth_plan</t>
-  </si>
-  <si>
-    <t>Develop a birth plan to ensure readiness for the arrival of the unborn baby</t>
-  </si>
-  <si>
     <t>trimester2_choices</t>
   </si>
   <si>
@@ -445,18 +445,18 @@
     <t>Is she still experiencing any danger signs?</t>
   </si>
   <si>
+    <t>couselling_on_exclusive_breastfeeding</t>
+  </si>
+  <si>
+    <t>Give your baby breast milk only (exclusive breastfeeding) for the first six months and continue breastfeeding for the first two years for good health</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
-    <t>couselling_on_exclusive_breastfeeding</t>
-  </si>
-  <si>
     <t>danger_signs_question_note</t>
   </si>
   <si>
-    <t>Give your baby breast milk only (exclusive breastfeeding) for the first six months and continue breastfeeding for the first two years for good health</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please indicate which danger signs ${patient_short_name} is experiencing. </t>
   </si>
   <si>
@@ -472,36 +472,36 @@
     <t>Heart condition</t>
   </si>
   <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
     <t>fever</t>
   </si>
   <si>
     <t>Fever</t>
   </si>
   <si>
-    <t>asthma</t>
-  </si>
-  <si>
-    <t>Asthma</t>
-  </si>
-  <si>
     <t>high_blood_pressure</t>
   </si>
   <si>
     <t>High blood pressure</t>
   </si>
   <si>
+    <t>known_diabetes</t>
+  </si>
+  <si>
+    <t>Known diabetes</t>
+  </si>
+  <si>
     <t>severe_headache</t>
   </si>
   <si>
     <t>Severe headache</t>
   </si>
   <si>
-    <t>known_diabetes</t>
-  </si>
-  <si>
-    <t>Known diabetes</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -514,28 +514,28 @@
     <t>Vaginal bleeding</t>
   </si>
   <si>
+    <t>hiv_statuses</t>
+  </si>
+  <si>
+    <t>known</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>vaginal_discharge</t>
   </si>
   <si>
-    <t>hiv_statuses</t>
-  </si>
-  <si>
-    <t>known</t>
-  </si>
-  <si>
     <t>Foul smelling vaginal discharge</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>fp_methods</t>
   </si>
   <si>
     <t>convulsion</t>
   </si>
   <si>
     <t>Convulsions</t>
-  </si>
-  <si>
-    <t>fp_methods</t>
   </si>
   <si>
     <t>r_danger_sign_present</t>
@@ -570,66 +570,66 @@
     <t>../danger_sign_present = 'yes' or ../r_danger_sign_present = 'yes'</t>
   </si>
   <si>
+    <t>Combined oral contraceptives</t>
+  </si>
+  <si>
+    <t>Progesterone only pills</t>
+  </si>
+  <si>
     <t>refer_patient_note_2</t>
   </si>
   <si>
     <t xml:space="preserve">Please advise her to do so and accompany her if possible. </t>
   </si>
   <si>
+    <t>Injectibles</t>
+  </si>
+  <si>
+    <t>Implants (1 rod)</t>
+  </si>
+  <si>
+    <t>Implants (2 rods)</t>
+  </si>
+  <si>
     <t>custom_translations</t>
   </si>
   <si>
-    <t>Combined oral contraceptives</t>
-  </si>
-  <si>
-    <t>Progesterone only pills</t>
-  </si>
-  <si>
-    <t>Injectibles</t>
+    <t>IUD</t>
+  </si>
+  <si>
+    <t>Condoms</t>
+  </si>
+  <si>
+    <t>Tubal ligation</t>
+  </si>
+  <si>
+    <t>Cycle beads</t>
   </si>
   <si>
     <t>select_one translate_woman_label</t>
   </si>
   <si>
-    <t>Implants (1 rod)</t>
-  </si>
-  <si>
     <t>custom_woman_label_translator</t>
   </si>
   <si>
-    <t>Implants (2 rods)</t>
-  </si>
-  <si>
     <t>"woman"</t>
   </si>
   <si>
-    <t>IUD</t>
-  </si>
-  <si>
-    <t>Condoms</t>
+    <t>reasons_not_on_fp</t>
+  </si>
+  <si>
+    <t>Wants to get pregnant</t>
   </si>
   <si>
     <t>custom_woman_label</t>
   </si>
   <si>
-    <t>Tubal ligation</t>
-  </si>
-  <si>
-    <t>Cycle beads</t>
+    <t>Did not want FP</t>
   </si>
   <si>
     <t>jr:choice-name(${custom_woman_label_translator},'${custom_woman_label_translator}')</t>
   </si>
   <si>
-    <t>reasons_not_on_fp</t>
-  </si>
-  <si>
-    <t>Wants to get pregnant</t>
-  </si>
-  <si>
-    <t>Did not want FP</t>
-  </si>
-  <si>
     <t>follow_up_methods</t>
   </si>
   <si>
@@ -645,16 +645,19 @@
     <t>In person</t>
   </si>
   <si>
+    <t>"woman-start"</t>
+  </si>
+  <si>
+    <t>custom_woman_start_label</t>
+  </si>
+  <si>
     <t>by_phone</t>
   </si>
   <si>
     <t>By phone</t>
   </si>
   <si>
-    <t>"woman-start"</t>
-  </si>
-  <si>
-    <t>custom_woman_start_label</t>
+    <t>jr:choice-name(${custom_woman_start_label_translator},'${custom_woman_start_label_translator}')</t>
   </si>
   <si>
     <t>reasons_for_missing_visit</t>
@@ -666,9 +669,6 @@
     <t>She was not reminded</t>
   </si>
   <si>
-    <t>jr:choice-name(${custom_woman_start_label_translator},'${custom_woman_start_label_translator}')</t>
-  </si>
-  <si>
     <t>travelled</t>
   </si>
   <si>
@@ -852,37 +852,37 @@
     <t>__patient_uuid</t>
   </si>
   <si>
-    <t>../../inputs/contact/_id</t>
+    <t>../../../inputs/contact/_id</t>
   </si>
   <si>
     <t>__patient_id</t>
   </si>
   <si>
-    <t>../../inputs/contact/patient_id</t>
+    <t>../../../inputs/contact/patient_id</t>
   </si>
   <si>
     <t>__household_uuid</t>
   </si>
   <si>
-    <t>../../inputs/contact/parent/_id</t>
+    <t>../../../inputs/contact/parent/_id</t>
   </si>
   <si>
     <t>__source</t>
   </si>
   <si>
-    <t>../../inputs/source</t>
+    <t>../../../inputs/source</t>
   </si>
   <si>
     <t>__source_id</t>
   </si>
   <si>
-    <t>../../inputs/source_id</t>
+    <t>../../../inputs/source_id</t>
   </si>
   <si>
     <t>__delivery_uuid</t>
   </si>
   <si>
-    <t>../../inputs/delivery_uuid</t>
+    <t>../../../inputs/delivery_uuid</t>
   </si>
 </sst>
 </file>
@@ -900,6 +900,11 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
     </font>
     <font>
       <b/>
@@ -908,11 +913,6 @@
       <name val="Calibri"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -953,6 +953,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
@@ -961,12 +967,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1025,14 +1025,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF8E7CC3"/>
+        <bgColor rgb="FF8E7CC3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8E7CC3"/>
-        <bgColor rgb="FF8E7CC3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1046,105 +1046,105 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="12" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="13" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="10" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="13" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -1154,28 +1154,28 @@
     <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="15" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1242,120 +1242,120 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
+      <c r="AA1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>36</v>
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1365,10 +1365,10 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
@@ -1396,14 +1396,14 @@
       <c r="AJ2" s="12"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -1432,7 +1432,7 @@
       <c r="AB3" s="9"/>
       <c r="AC3" s="9"/>
       <c r="AD3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE3" s="9"/>
       <c r="AF3" s="9"/>
@@ -1442,14 +1442,14 @@
       <c r="AJ3" s="12"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1486,14 +1486,14 @@
       <c r="AJ4" s="12"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>59</v>
+      <c r="A5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1530,14 +1530,14 @@
       <c r="AJ5" s="12"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1574,14 +1574,14 @@
       <c r="AJ6" s="12"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>66</v>
+      <c r="A7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1592,7 +1592,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -1620,14 +1620,14 @@
       <c r="AJ7" s="12"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
+      <c r="A8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1664,14 +1664,14 @@
       <c r="AJ8" s="12"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>73</v>
+      <c r="A9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1708,14 +1708,14 @@
       <c r="AJ9" s="12"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>76</v>
+      <c r="A10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1752,14 +1752,14 @@
       <c r="AJ10" s="12"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>82</v>
+      <c r="A11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1798,14 +1798,14 @@
       <c r="AJ11" s="12"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>84</v>
+      <c r="A12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1842,14 +1842,14 @@
       <c r="AJ12" s="12"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>86</v>
+      <c r="A13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1886,14 +1886,14 @@
       <c r="AJ13" s="12"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>66</v>
+      <c r="A14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1925,19 +1925,19 @@
       <c r="AE14" s="9"/>
       <c r="AF14" s="9"/>
       <c r="AG14" s="9"/>
-      <c r="AH14" s="29"/>
-      <c r="AI14" s="29"/>
-      <c r="AJ14" s="29"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>86</v>
+      <c r="A15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -1974,14 +1974,14 @@
       <c r="AJ15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
+      <c r="A16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -2018,14 +2018,14 @@
       <c r="AJ16" s="12"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>89</v>
+      <c r="A17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -2062,14 +2062,14 @@
       <c r="AJ17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
+      <c r="A18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -2106,11 +2106,11 @@
       <c r="AJ18" s="12"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>63</v>
+      <c r="B19" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2148,11 +2148,11 @@
       <c r="AJ19" s="12"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>86</v>
+      <c r="B20" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2190,11 +2190,11 @@
       <c r="AJ20" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>86</v>
+      <c r="B21" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -2232,11 +2232,11 @@
       <c r="AJ21" s="12"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>63</v>
+      <c r="B22" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2274,11 +2274,11 @@
       <c r="AJ22" s="12"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>36</v>
+      <c r="B23" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2362,7 +2362,7 @@
       <c r="AD25" s="33"/>
       <c r="AE25" s="33"/>
       <c r="AF25" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG25" s="33"/>
       <c r="AH25" s="35"/>
@@ -2410,7 +2410,7 @@
       <c r="AD26" s="33"/>
       <c r="AE26" s="33"/>
       <c r="AF26" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG26" s="33"/>
       <c r="AH26" s="35"/>
@@ -2422,7 +2422,7 @@
         <v>94</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
@@ -2434,7 +2434,7 @@
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
       <c r="J27" s="33" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K27" s="33"/>
       <c r="L27" s="33"/>
@@ -2460,7 +2460,7 @@
       <c r="AD27" s="33"/>
       <c r="AE27" s="33"/>
       <c r="AF27" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG27" s="33"/>
       <c r="AH27" s="35"/>
@@ -2508,7 +2508,7 @@
       <c r="AD28" s="33"/>
       <c r="AE28" s="33"/>
       <c r="AF28" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG28" s="33"/>
       <c r="AH28" s="35"/>
@@ -2520,7 +2520,7 @@
         <v>94</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>96</v>
@@ -2543,7 +2543,7 @@
       <c r="S29" s="33"/>
       <c r="T29" s="33"/>
       <c r="U29" s="34" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="V29" s="33"/>
       <c r="W29" s="33"/>
@@ -2556,7 +2556,7 @@
       <c r="AD29" s="33"/>
       <c r="AE29" s="33"/>
       <c r="AF29" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG29" s="33"/>
       <c r="AH29" s="35"/>
@@ -2568,7 +2568,7 @@
         <v>94</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>96</v>
@@ -2591,7 +2591,7 @@
       <c r="S30" s="33"/>
       <c r="T30" s="33"/>
       <c r="U30" s="34" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
@@ -2604,7 +2604,7 @@
       <c r="AD30" s="33"/>
       <c r="AE30" s="33"/>
       <c r="AF30" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG30" s="33"/>
       <c r="AH30" s="35"/>
@@ -2616,7 +2616,7 @@
         <v>94</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C31" s="34" t="s">
         <v>96</v>
@@ -2639,7 +2639,7 @@
       <c r="S31" s="33"/>
       <c r="T31" s="33"/>
       <c r="U31" s="34" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="V31" s="33"/>
       <c r="W31" s="33"/>
@@ -2652,7 +2652,7 @@
       <c r="AD31" s="33"/>
       <c r="AE31" s="33"/>
       <c r="AF31" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG31" s="33"/>
       <c r="AH31" s="37"/>
@@ -2664,7 +2664,7 @@
         <v>94</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>96</v>
@@ -2687,7 +2687,7 @@
       <c r="S32" s="33"/>
       <c r="T32" s="33"/>
       <c r="U32" s="34" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="V32" s="33"/>
       <c r="W32" s="33"/>
@@ -2700,7 +2700,7 @@
       <c r="AD32" s="33"/>
       <c r="AE32" s="33"/>
       <c r="AF32" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG32" s="33"/>
       <c r="AH32" s="37"/>
@@ -2719,13 +2719,13 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="39" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
@@ -2736,7 +2736,7 @@
       <c r="J34" s="41"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M34" s="41"/>
       <c r="N34" s="41"/>
@@ -2780,7 +2780,7 @@
       <c r="H35" s="41"/>
       <c r="I35" s="41"/>
       <c r="J35" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K35" s="41"/>
       <c r="L35" s="41"/>
@@ -2826,7 +2826,7 @@
       <c r="H36" s="41"/>
       <c r="I36" s="41"/>
       <c r="J36" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K36" s="41"/>
       <c r="L36" s="41"/>
@@ -2857,10 +2857,10 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>147</v>
@@ -2896,7 +2896,7 @@
       <c r="AD37" s="41"/>
       <c r="AE37" s="41"/>
       <c r="AF37" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG37" s="41"/>
       <c r="AH37" s="42"/>
@@ -2908,10 +2908,10 @@
         <v>138</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
@@ -2920,7 +2920,7 @@
       <c r="H38" s="41"/>
       <c r="I38" s="41"/>
       <c r="J38" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K38" s="40" t="s">
         <v>148</v>
@@ -2956,10 +2956,10 @@
         <v>138</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
@@ -2968,7 +2968,7 @@
       <c r="H39" s="41"/>
       <c r="I39" s="41"/>
       <c r="J39" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K39" s="40" t="s">
         <v>148</v>
@@ -3016,7 +3016,7 @@
       <c r="H40" s="41"/>
       <c r="I40" s="41"/>
       <c r="J40" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K40" s="40" t="s">
         <v>148</v>
@@ -3052,10 +3052,10 @@
         <v>138</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
@@ -3064,7 +3064,7 @@
       <c r="H41" s="41"/>
       <c r="I41" s="41"/>
       <c r="J41" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K41" s="40" t="s">
         <v>148</v>
@@ -3100,10 +3100,10 @@
         <v>138</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
@@ -3112,7 +3112,7 @@
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="41" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="K42" s="40" t="s">
         <v>148</v>
@@ -3184,7 +3184,7 @@
       <c r="AD43" s="41"/>
       <c r="AE43" s="41"/>
       <c r="AF43" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG43" s="41"/>
       <c r="AH43" s="42"/>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="39" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B44" s="39" t="s">
         <v>176</v>
@@ -3232,7 +3232,7 @@
       <c r="AD44" s="41"/>
       <c r="AE44" s="41"/>
       <c r="AF44" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG44" s="41"/>
       <c r="AH44" s="44"/>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B45" s="39" t="s">
         <v>179</v>
@@ -3280,7 +3280,7 @@
       <c r="AD45" s="41"/>
       <c r="AE45" s="41"/>
       <c r="AF45" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG45" s="41"/>
       <c r="AH45" s="44"/>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D46" s="41"/>
       <c r="E46" s="41"/>
@@ -3328,7 +3328,7 @@
       <c r="AD46" s="41"/>
       <c r="AE46" s="41"/>
       <c r="AF46" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG46" s="41"/>
       <c r="AH46" s="42"/>
@@ -3337,10 +3337,10 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="39" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>96</v>
@@ -3354,7 +3354,7 @@
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
       <c r="L47" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M47" s="41"/>
       <c r="N47" s="41"/>
@@ -3376,7 +3376,7 @@
       <c r="AD47" s="41"/>
       <c r="AE47" s="41"/>
       <c r="AF47" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG47" s="41"/>
       <c r="AH47" s="45"/>
@@ -3385,10 +3385,10 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="39" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>96</v>
@@ -3411,7 +3411,7 @@
       <c r="S48" s="41"/>
       <c r="T48" s="41"/>
       <c r="U48" s="40" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="V48" s="41"/>
       <c r="W48" s="41"/>
@@ -3434,7 +3434,7 @@
         <v>94</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>96</v>
@@ -3457,7 +3457,7 @@
       <c r="S49" s="41"/>
       <c r="T49" s="41"/>
       <c r="U49" s="40" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="V49" s="41"/>
       <c r="W49" s="41"/>
@@ -3503,7 +3503,7 @@
       <c r="S50" s="41"/>
       <c r="T50" s="41"/>
       <c r="U50" s="40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="V50" s="41"/>
       <c r="W50" s="41"/>
@@ -3526,7 +3526,7 @@
         <v>94</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>96</v>
@@ -3549,7 +3549,7 @@
       <c r="S51" s="41"/>
       <c r="T51" s="41"/>
       <c r="U51" s="40" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="V51" s="41"/>
       <c r="W51" s="41"/>
@@ -3655,16 +3655,16 @@
       <c r="F54" s="30"/>
       <c r="AF54" s="30"/>
       <c r="AG54" s="30"/>
-      <c r="AH54" s="48"/>
-      <c r="AI54" s="48"/>
-      <c r="AJ54" s="48"/>
+      <c r="AH54" s="47"/>
+      <c r="AI54" s="47"/>
+      <c r="AJ54" s="47"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="49" t="s">
-        <v>49</v>
+      <c r="A55" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="48" t="s">
+        <v>58</v>
       </c>
       <c r="C55" s="50" t="s">
         <v>96</v>
@@ -3678,7 +3678,7 @@
       <c r="J55" s="51"/>
       <c r="K55" s="51"/>
       <c r="L55" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M55" s="51"/>
       <c r="N55" s="51"/>
@@ -3700,7 +3700,7 @@
       <c r="AD55" s="51"/>
       <c r="AE55" s="51"/>
       <c r="AF55" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG55" s="50"/>
       <c r="AH55" s="53"/>
@@ -3708,7 +3708,7 @@
       <c r="AJ55" s="53"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="54" t="s">
@@ -3754,7 +3754,7 @@
       <c r="AJ56" s="53"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="54" t="s">
@@ -3800,7 +3800,7 @@
       <c r="AJ57" s="53"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B58" s="54" t="s">
@@ -3846,7 +3846,7 @@
       <c r="AJ58" s="53"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B59" s="54" t="s">
@@ -3892,7 +3892,7 @@
       <c r="AJ59" s="53"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B60" s="54" t="s">
@@ -3938,7 +3938,7 @@
       <c r="AJ60" s="53"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B61" s="54" t="s">
@@ -3984,7 +3984,7 @@
       <c r="AJ61" s="53"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B62" s="54" t="s">
@@ -4030,7 +4030,7 @@
       <c r="AJ62" s="53"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B63" s="54" t="s">
@@ -4077,7 +4077,7 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="56" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B64" s="56" t="s">
         <v>274</v>
@@ -4120,7 +4120,7 @@
       <c r="AJ64" s="53"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B65" s="54" t="s">
@@ -4144,7 +4144,7 @@
       <c r="R65" s="51"/>
       <c r="S65" s="51"/>
       <c r="T65" s="51"/>
-      <c r="U65" s="50" t="s">
+      <c r="U65" s="53" t="s">
         <v>276</v>
       </c>
       <c r="V65" s="51"/>
@@ -4164,7 +4164,7 @@
       <c r="AJ65" s="53"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B66" s="54" t="s">
@@ -4188,7 +4188,7 @@
       <c r="R66" s="51"/>
       <c r="S66" s="51"/>
       <c r="T66" s="51"/>
-      <c r="U66" s="50" t="s">
+      <c r="U66" s="53" t="s">
         <v>278</v>
       </c>
       <c r="V66" s="51"/>
@@ -4208,7 +4208,7 @@
       <c r="AJ66" s="53"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B67" s="54" t="s">
@@ -4232,7 +4232,7 @@
       <c r="R67" s="51"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
-      <c r="U67" s="50" t="s">
+      <c r="U67" s="53" t="s">
         <v>280</v>
       </c>
       <c r="V67" s="51"/>
@@ -4252,7 +4252,7 @@
       <c r="AJ67" s="53"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B68" s="54" t="s">
@@ -4276,7 +4276,7 @@
       <c r="R68" s="51"/>
       <c r="S68" s="51"/>
       <c r="T68" s="51"/>
-      <c r="U68" s="50" t="s">
+      <c r="U68" s="53" t="s">
         <v>282</v>
       </c>
       <c r="V68" s="51"/>
@@ -4296,7 +4296,7 @@
       <c r="AJ68" s="53"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="49" t="s">
+      <c r="A69" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B69" s="54" t="s">
@@ -4320,7 +4320,7 @@
       <c r="R69" s="51"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
-      <c r="U69" s="50" t="s">
+      <c r="U69" s="53" t="s">
         <v>284</v>
       </c>
       <c r="V69" s="51"/>
@@ -4340,7 +4340,7 @@
       <c r="AJ69" s="53"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B70" s="54" t="s">
@@ -4364,7 +4364,7 @@
       <c r="R70" s="51"/>
       <c r="S70" s="51"/>
       <c r="T70" s="51"/>
-      <c r="U70" s="50" t="s">
+      <c r="U70" s="52" t="s">
         <v>286</v>
       </c>
       <c r="V70" s="51"/>
@@ -4430,7 +4430,7 @@
         <v>93</v>
       </c>
       <c r="B72" s="56" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C72" s="53"/>
       <c r="D72" s="57"/>
@@ -4495,56 +4495,56 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -4568,13 +4568,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -4597,9 +4597,9 @@
       <c r="V3" s="25"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -4621,25 +4621,25 @@
       <c r="V4" s="25"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>77</v>
+      <c r="A5" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>81</v>
+      <c r="A6" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -4850,87 +4850,87 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11">
         <f>NOW()</f>
-        <v>43747.52795</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="10" t="s">
+        <v>43748.59599</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
+      <c r="E2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -4955,57 +4955,57 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -5030,13 +5030,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -5086,13 +5086,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
@@ -5117,13 +5117,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
@@ -5148,13 +5148,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>117</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
@@ -5179,13 +5179,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -5210,13 +5210,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -5266,13 +5266,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -5297,10 +5297,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>126</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>127</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>129</v>
@@ -5390,13 +5390,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -5421,13 +5421,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -5480,10 +5480,10 @@
         <v>137</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -5511,7 +5511,7 @@
         <v>137</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>126</v>
@@ -5604,10 +5604,10 @@
         <v>137</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
@@ -5635,10 +5635,10 @@
         <v>137</v>
       </c>
       <c r="B23" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="25" t="s">
         <v>144</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
@@ -5722,10 +5722,10 @@
         <v>149</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
@@ -5784,10 +5784,10 @@
         <v>149</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>168</v>
-      </c>
       <c r="C31" s="25" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -5899,13 +5899,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -5955,115 +5955,115 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B43" t="s">
         <v>162</v>
@@ -6080,26 +6080,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -6109,82 +6109,82 @@
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
-      <c r="T48" s="14"/>
-      <c r="U48" s="14"/>
-      <c r="V48" s="14"/>
-      <c r="W48" s="14"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
+      <c r="B49" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
     </row>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C51" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B52" t="s">
         <v>215</v>
@@ -6195,7 +6195,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
         <v>217</v>
@@ -6206,7 +6206,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s">
         <v>219</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B55" t="s">
         <v>221</v>
@@ -6228,7 +6228,7 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
         <v>162</v>
@@ -6239,102 +6239,102 @@
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="27" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="27" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="27" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="27" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="27" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="27" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="27" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="27" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="27" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6369,8 +6369,8 @@
       <c r="B72" t="s">
         <v>247</v>
       </c>
-      <c r="C72" s="47" t="s">
-        <v>200</v>
+      <c r="C72" s="49" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">

</xml_diff>